<commit_message>
Thema keuze verbetering gedocumenteerd
</commit_message>
<xml_diff>
--- a/Documentatie/Feedback Sheet.xlsx
+++ b/Documentatie/Feedback Sheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B990ABC8-A67D-4733-81AC-FD39FC0E8518}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C513EB-A65D-4796-915B-248C52708AC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ontvangen Feedback" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Onderwerp</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Het logo ziet er tot nu toe goed uit, probeer ook wat met kleur te werken. Misschien slim om ook met andere fonts te proberen. Pas wel op dat je er niet te veel tijd in steekt want het is maar een klein onderdeel.</t>
+  </si>
+  <si>
+    <t>Thema onderzoek besproken</t>
   </si>
 </sst>
 </file>
@@ -205,7 +208,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -545,21 +548,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" customWidth="1"/>
-    <col min="6" max="6" width="185.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="185.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -579,7 +582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -599,7 +602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -619,7 +622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -639,7 +642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -659,7 +662,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -667,7 +670,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
@@ -675,7 +678,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
@@ -683,7 +686,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
@@ -691,7 +694,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -699,7 +702,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
@@ -707,7 +710,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
@@ -715,7 +718,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -723,7 +726,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
@@ -731,7 +734,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
@@ -739,7 +742,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
@@ -747,7 +750,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
@@ -755,7 +758,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
@@ -763,7 +766,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -771,7 +774,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6"/>
@@ -779,7 +782,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
@@ -787,7 +790,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
@@ -795,7 +798,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
@@ -803,7 +806,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
@@ -811,7 +814,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
@@ -819,7 +822,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
@@ -827,7 +830,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
@@ -835,7 +838,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
@@ -843,7 +846,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>
@@ -851,7 +854,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="6"/>
@@ -859,7 +862,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="7"/>
       <c r="C31" s="8"/>
@@ -880,20 +883,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1ED5DB6-57AF-4F6E-A1E3-6C52533493D6}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="75.109375" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="75.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -910,7 +913,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>43206</v>
       </c>
@@ -927,7 +930,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>43206</v>
       </c>
@@ -944,7 +947,7 @@
         <v>43213</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>43213</v>
       </c>
@@ -961,103 +964,117 @@
         <v>43220</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>43227</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="12">
+        <v>43227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
     </row>
   </sheetData>

</xml_diff>